<commit_message>
Save calculated column formula in table field
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <x:si>
     <x:t>FName</x:t>
   </x:si>
@@ -31,6 +31,9 @@
   </x:si>
   <x:si>
     <x:t>Income</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Age</x:t>
   </x:si>
   <x:si>
     <x:t>Table Headers</x:t>
@@ -76,9 +79,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:numFmts count="2">
+  <x:numFmts count="3">
     <x:numFmt numFmtId="0" formatCode=""/>
     <x:numFmt numFmtId="165" formatCode="$ #,##0"/>
+    <x:numFmt numFmtId="166" formatCode="0.00"/>
   </x:numFmts>
   <x:fonts count="2">
     <x:font>
@@ -289,7 +293,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="25">
+  <x:cellStyleXfs count="26">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -341,6 +345,9 @@
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -366,7 +373,7 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="17">
+  <x:cellXfs count="18">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -432,6 +439,10 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -443,21 +454,24 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:F6" totalsRowCount="1">
-  <x:autoFilter ref="B2:F5"/>
-  <x:tableColumns count="5">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B2:G6" totalsRowCount="1">
+  <x:autoFilter ref="B2:G5"/>
+  <x:tableColumns count="6">
     <x:tableColumn id="1" name="FName" totalsRowLabel="Sum Of Income"/>
     <x:tableColumn id="2" name="LName"/>
     <x:tableColumn id="3" name="Outcast"/>
     <x:tableColumn id="4" name="DOB"/>
     <x:tableColumn id="5" name="Income" totalsRowFunction="sum"/>
+    <x:tableColumn id="6" name="Age" totalsRowFunction="average">
+      <x:calculatedColumnFormula>(DATE(2017, 10, 3) - E3) / 365</x:calculatedColumnFormula>
+    </x:tableColumn>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Headers" displayName="Headers" ref="H2:H8" totalsRowCount="1">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Headers" displayName="Headers" ref="I2:I9" totalsRowCount="1">
   <x:tableColumns count="1">
     <x:tableColumn id="1" name="Table Headers" totalsRowFunction="custom">
       <x:totalsRowFormula>CONCATENATE("Count: ", CountA(Headers[Table Headers]))</x:totalsRowFormula>
@@ -468,7 +482,7 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table2" displayName="Table2" ref="J2:J5" totalsRowShown="0">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table2" displayName="Table2" ref="K2:K5" totalsRowShown="0">
   <x:tableColumns count="1">
     <x:tableColumn id="1" name="Names"/>
   </x:tableColumns>
@@ -477,21 +491,24 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table11" displayName="Table11" ref="B2:F6" totalsRowCount="1">
-  <x:autoFilter ref="B2:F5"/>
-  <x:tableColumns count="5">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table11" displayName="Table11" ref="B2:G6" totalsRowCount="1">
+  <x:autoFilter ref="B2:G5"/>
+  <x:tableColumns count="6">
     <x:tableColumn id="1" name="FName" totalsRowLabel="Sum Of Income"/>
     <x:tableColumn id="2" name="LName"/>
     <x:tableColumn id="3" name="Outcast"/>
     <x:tableColumn id="4" name="DOB"/>
     <x:tableColumn id="5" name="Income" totalsRowFunction="sum"/>
+    <x:tableColumn id="6" name="Age" totalsRowFunction="average">
+      <x:calculatedColumnFormula>(DATE(2017, 10, 3) - E3) / 365</x:calculatedColumnFormula>
+    </x:tableColumn>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Headers1" displayName="Headers1" ref="H2:H8" totalsRowCount="1">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Headers1" displayName="Headers1" ref="I2:I9" totalsRowCount="1">
   <x:tableColumns count="1">
     <x:tableColumn id="1" name="Table Headers" totalsRowFunction="custom">
       <x:totalsRowFormula>CONCATENATE("Count: ", CountA(Headers[Table Headers]))</x:totalsRowFormula>
@@ -502,7 +519,7 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table21" displayName="Table21" ref="J2:J5" totalsRowShown="0">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table21" displayName="Table21" ref="K2:K5" totalsRowShown="0">
   <x:tableColumns count="1">
     <x:tableColumn id="1" name="Names"/>
   </x:tableColumns>
@@ -810,13 +827,14 @@
     <x:col min="4" max="4" width="11.155425" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="10.140625" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="10.895425" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="3.710625" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="16.725425" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="3.710625" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="13.830625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="18.300625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="3.710625" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="16.725425" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="3.710625" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="13.830625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:10">
+    <x:row r="2" spans="1:11">
       <x:c r="B2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -832,19 +850,22 @@
       <x:c r="F2" s="16" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="J2" s="0" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:10">
+      <x:c r="K2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
       <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D3" s="0" t="b">
         <x:v>1</x:v>
@@ -855,19 +876,22 @@
       <x:c r="F3" s="16" t="n">
         <x:v>2000</x:v>
       </x:c>
-      <x:c r="H3" s="0" t="s">
+      <x:c r="G3" s="17">
+        <x:f>(DATE(2017, 10, 3) - E3) / 365</x:f>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:10">
+      <x:c r="K3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
       <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D4" s="0" t="b">
         <x:v>0</x:v>
@@ -878,19 +902,22 @@
       <x:c r="F4" s="16" t="n">
         <x:v>40000</x:v>
       </x:c>
-      <x:c r="H4" s="0" t="s">
+      <x:c r="G4" s="17">
+        <x:f>(DATE(2017, 10, 3) - E4) / 365</x:f>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="J4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:10">
+      <x:c r="K4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
       <x:c r="B5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D5" s="0" t="b">
         <x:v>0</x:v>
@@ -901,32 +928,43 @@
       <x:c r="F5" s="16" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="H5" s="0" t="s">
+      <x:c r="G5" s="17">
+        <x:f>(DATE(2017, 10, 3) - E5) / 365</x:f>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="J5" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:10">
+      <x:c r="K5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
       <x:c r="B6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E6" s="15" t="s"/>
       <x:c r="F6" s="16" t="n">
         <x:f>SUBTOTAL(109,[Income])</x:f>
       </x:c>
-      <x:c r="H6" s="0" t="s">
+      <x:c r="G6" s="17">
+        <x:f>SUBTOTAL(101,[Age])</x:f>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:10">
-      <x:c r="H7" s="0" t="s">
+    <x:row r="7" spans="1:11">
+      <x:c r="I7" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:10">
-      <x:c r="H8" s="0">
+    <x:row r="8" spans="1:11">
+      <x:c r="I8" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="I9" s="0">
         <x:f>CONCATENATE("Count: ", CountA(Headers[Table Headers]))</x:f>
       </x:c>
     </x:row>
@@ -948,7 +986,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:J8"/>
+  <x:dimension ref="A1:K9"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -960,13 +998,14 @@
     <x:col min="4" max="4" width="11.155425" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="10.140625" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="10.895425" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="3.710625" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="16.725425" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="3.710625" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="13.830625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="18.300625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="3.710625" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="16.725425" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="3.710625" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="13.830625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="2" spans="1:10">
+    <x:row r="2" spans="1:11">
       <x:c r="B2" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -982,19 +1021,22 @@
       <x:c r="F2" s="16" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="J2" s="0" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:10">
+      <x:c r="K2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:11">
       <x:c r="B3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D3" s="0" t="b">
         <x:v>1</x:v>
@@ -1005,19 +1047,22 @@
       <x:c r="F3" s="16" t="n">
         <x:v>2000</x:v>
       </x:c>
-      <x:c r="H3" s="0" t="s">
+      <x:c r="G3" s="17">
+        <x:f>(DATE(2017, 10, 3) - E3) / 365</x:f>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:10">
+      <x:c r="K3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:11">
       <x:c r="B4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D4" s="0" t="b">
         <x:v>0</x:v>
@@ -1028,19 +1073,22 @@
       <x:c r="F4" s="16" t="n">
         <x:v>40000</x:v>
       </x:c>
-      <x:c r="H4" s="0" t="s">
+      <x:c r="G4" s="17">
+        <x:f>(DATE(2017, 10, 3) - E4) / 365</x:f>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="J4" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:10">
+      <x:c r="K4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:11">
       <x:c r="B5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D5" s="0" t="b">
         <x:v>0</x:v>
@@ -1051,32 +1099,43 @@
       <x:c r="F5" s="16" t="n">
         <x:v>10000</x:v>
       </x:c>
-      <x:c r="H5" s="0" t="s">
+      <x:c r="G5" s="17">
+        <x:f>(DATE(2017, 10, 3) - E5) / 365</x:f>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="J5" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:10">
+      <x:c r="K5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:11">
       <x:c r="B6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E6" s="15" t="s"/>
       <x:c r="F6" s="16">
         <x:f>SUBTOTAL(109,[Income])</x:f>
       </x:c>
-      <x:c r="H6" s="0" t="s">
+      <x:c r="G6" s="17">
+        <x:f>SUBTOTAL(101,[Age])</x:f>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:10">
-      <x:c r="H7" s="0" t="s">
+    <x:row r="7" spans="1:11">
+      <x:c r="I7" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:10">
-      <x:c r="H8" s="0">
+    <x:row r="8" spans="1:11">
+      <x:c r="I8" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:11">
+      <x:c r="I9" s="0">
         <x:f>CONCATENATE("Count: ", CountA(Headers[Table Headers]))</x:f>
       </x:c>
     </x:row>
@@ -1121,7 +1180,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:6">
       <x:c r="B2" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s"/>
       <x:c r="D2" s="2" t="s"/>
@@ -1147,10 +1206,10 @@
     </x:row>
     <x:row r="4" spans="1:6">
       <x:c r="B4" s="7" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C4" s="8" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="D4" s="8" t="b">
         <x:v>1</x:v>
@@ -1164,10 +1223,10 @@
     </x:row>
     <x:row r="5" spans="1:6">
       <x:c r="B5" s="7" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C5" s="8" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="D5" s="8" t="b">
         <x:v>0</x:v>
@@ -1181,10 +1240,10 @@
     </x:row>
     <x:row r="6" spans="1:6">
       <x:c r="B6" s="11" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C6" s="12" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="D6" s="12" t="b">
         <x:v>0</x:v>

</xml_diff>

<commit_message>
Update reference files (fills with patternType="none" removed)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
@@ -427,21 +427,12 @@
   <x:dxfs count="3">
     <x:dxf>
       <x:numFmt numFmtId="15" formatCode="d-MMM-yy"/>
-      <x:fill>
-        <x:patternFill patternType="none"/>
-      </x:fill>
     </x:dxf>
     <x:dxf>
       <x:numFmt numFmtId="164" formatCode="$ #,##0"/>
-      <x:fill>
-        <x:patternFill patternType="none"/>
-      </x:fill>
     </x:dxf>
     <x:dxf>
       <x:numFmt numFmtId="165" formatCode="0.00"/>
-      <x:fill>
-        <x:patternFill patternType="none"/>
-      </x:fill>
     </x:dxf>
   </x:dxfs>
 </x:styleSheet>

</xml_diff>

<commit_message>
Copies of tables should have RelId default to null
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/CopyingWorksheets.xlsx
@@ -1137,9 +1137,9 @@
     <x:firstFooter/>
   </x:headerFooter>
   <x:tableParts count="3">
-    <x:tablePart r:id="rId5"/>
-    <x:tablePart r:id="rId7"/>
-    <x:tablePart r:id="rId8"/>
+    <x:tablePart r:id="rId12"/>
+    <x:tablePart r:id="rId13"/>
+    <x:tablePart r:id="rId14"/>
   </x:tableParts>
 </x:worksheet>
 </file>

</xml_diff>